<commit_message>
Fix names in member list
</commit_message>
<xml_diff>
--- a/20231114_SEATRAC_Member_PubSearch.xlsx
+++ b/20231114_SEATRAC_Member_PubSearch.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27230"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid.sharepoint.com/sites/og_sea_trac/Shared Documents/Administration Core/Admin/Literature_Summary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid.sharepoint.com/sites/og_sea_trac/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A6C5638-BF08-4BC2-81E4-B93CD22EAB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3933DF6C-05C8-4CBD-9CE6-0FD158EA014D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="500" windowWidth="28620" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="35115" yWindow="1125" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - SEATRACMembership-Mem" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="217">
   <si>
     <t>Last Name</t>
   </si>
@@ -56,6 +56,180 @@
     <t>NOTES</t>
   </si>
   <si>
+    <t>Abdelaal</t>
+  </si>
+  <si>
+    <t>Hazem</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>Seattle Children's Research Institute</t>
+  </si>
+  <si>
+    <t>Postdoctoral Trainee (Lab-based or Clinical Fellow)</t>
+  </si>
+  <si>
+    <t>Abernethy</t>
+  </si>
+  <si>
+    <t>Neil</t>
+  </si>
+  <si>
+    <t>University of Washington</t>
+  </si>
+  <si>
+    <t>Associate Professor or Member</t>
+  </si>
+  <si>
+    <t>Aitchison</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Professor or Member</t>
+  </si>
+  <si>
+    <t>Andersen-Nissen</t>
+  </si>
+  <si>
+    <t>Erica</t>
+  </si>
+  <si>
+    <t>Fred Hutchinson Cancer Research Center</t>
+  </si>
+  <si>
+    <t>Staff Scientist</t>
+  </si>
+  <si>
+    <t>Anterasian</t>
+  </si>
+  <si>
+    <t>Christine</t>
+  </si>
+  <si>
+    <t>Seattle Children's Hospital</t>
+  </si>
+  <si>
+    <t>Assistant Professor or Member</t>
+  </si>
+  <si>
+    <t>Attia</t>
+  </si>
+  <si>
+    <t>Engi</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Bedru</t>
+  </si>
+  <si>
+    <t>Eldana</t>
+  </si>
+  <si>
+    <t>Bender Ignacio</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Bergado</t>
+  </si>
+  <si>
+    <t>Monica</t>
+  </si>
+  <si>
+    <t>Relevant papers will include Ma S</t>
+  </si>
+  <si>
+    <t>Bhagwat</t>
+  </si>
+  <si>
+    <t>Amala</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Danae</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Brumwell</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Buckner</t>
+  </si>
+  <si>
+    <t>Frederick</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Cangelosi</t>
+  </si>
+  <si>
+    <t>Gerard</t>
+  </si>
+  <si>
+    <t>Celum</t>
+  </si>
+  <si>
+    <t>Connie</t>
+  </si>
+  <si>
+    <t>Chohan</t>
+  </si>
+  <si>
+    <t>Bhavna</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Acting or Clinical Instructor</t>
+  </si>
+  <si>
+    <t>Coler</t>
+  </si>
+  <si>
+    <t>Rhea</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Connolly</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Cowan</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Deshpande</t>
+  </si>
+  <si>
+    <t>Aditi</t>
+  </si>
+  <si>
+    <t>Seattle Chilren's Research Institute</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dewan </t>
   </si>
   <si>
@@ -71,66 +245,267 @@
     <t>Other</t>
   </si>
   <si>
+    <t>Duffy</t>
+  </si>
+  <si>
+    <t>Fergal</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Research Or Staff Scientist</t>
+  </si>
+  <si>
+    <t>Edlefsen</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Eldesouky</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Escudero</t>
+  </si>
+  <si>
+    <t>Jaclyn</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Erkang</t>
+  </si>
+  <si>
+    <t>Relevant papers will always include FS Buckner</t>
+  </si>
+  <si>
+    <t>Ferede</t>
+  </si>
+  <si>
+    <t>Debora</t>
+  </si>
+  <si>
+    <t>Relevant papers will include Coler RN</t>
+  </si>
+  <si>
+    <t>Fiore-Gartland</t>
+  </si>
+  <si>
+    <t>Gern</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Gerner</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Ghassemieh</t>
+  </si>
+  <si>
+    <t>Bijan</t>
+  </si>
+  <si>
     <t>Ginsburg</t>
   </si>
   <si>
     <t>Ann</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Professor or Member</t>
-  </si>
-  <si>
-    <t>Andersen-Nissen</t>
-  </si>
-  <si>
-    <t>Erica</t>
-  </si>
-  <si>
-    <t>Fred Hutchinson Cancer Research Center</t>
-  </si>
-  <si>
-    <t>Staff Scientist</t>
-  </si>
-  <si>
-    <t>Edlefsen</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>Research Or Staff Scientist</t>
-  </si>
-  <si>
-    <t>Fiore-Gartland</t>
-  </si>
-  <si>
-    <t>Andrew</t>
+    <t>Gonzalez-Reyes</t>
+  </si>
+  <si>
+    <t>Rebeca</t>
+  </si>
+  <si>
+    <t>Gottlieb</t>
+  </si>
+  <si>
+    <t>Geoffrey</t>
+  </si>
+  <si>
+    <t>Graham</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Grundner</t>
+  </si>
+  <si>
+    <t>Christoph</t>
+  </si>
+  <si>
+    <t>Harne</t>
+  </si>
+  <si>
+    <t>Rakhi</t>
+  </si>
+  <si>
+    <t>Relevant papers will always include Coler RN</t>
+  </si>
+  <si>
+    <t>Harrington</t>
+  </si>
+  <si>
+    <t>Whitney</t>
+  </si>
+  <si>
+    <t>Hawn</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t>Horne</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Iribarren</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Jaspan</t>
+  </si>
+  <si>
+    <t>Heather</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>John-Stewart</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Kaushansky</t>
+  </si>
+  <si>
+    <t>Alexis</t>
+  </si>
+  <si>
+    <t>Kerani</t>
+  </si>
+  <si>
+    <t>Roxanne</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Koelle</t>
   </si>
   <si>
     <t>Kublin</t>
   </si>
   <si>
-    <t>James</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
+    <t>LaCourse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sylvia </t>
+  </si>
+  <si>
+    <t>Liles</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Conrad</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Lutz</t>
+  </si>
+  <si>
+    <t>Barry</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>Shuyi</t>
+  </si>
+  <si>
+    <t>Need to search with Affiliation</t>
+  </si>
+  <si>
+    <t>Maerz</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Relevant papers will include Seshadri C</t>
+  </si>
+  <si>
+    <t>Mayanja-Kizza</t>
+  </si>
+  <si>
+    <t>Harriet</t>
+  </si>
+  <si>
+    <t>Makerere University</t>
+  </si>
+  <si>
+    <t>McDermott</t>
+  </si>
+  <si>
+    <t>Suzanne</t>
+  </si>
+  <si>
     <t>McElrath</t>
   </si>
   <si>
     <t>Margaret</t>
   </si>
   <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>Moritz</t>
   </si>
   <si>
@@ -143,385 +518,163 @@
     <t>Institute for Systems Biology</t>
   </si>
   <si>
+    <t>Narita</t>
+  </si>
+  <si>
+    <t>Masa</t>
+  </si>
+  <si>
+    <t>Public Health Seattle/King County</t>
+  </si>
+  <si>
+    <t>Masahiro</t>
+  </si>
+  <si>
+    <t>Nduba</t>
+  </si>
+  <si>
+    <t>Videlis</t>
+  </si>
+  <si>
+    <t>Kenya Medical Research Institute</t>
+  </si>
+  <si>
+    <t>Ngo</t>
+  </si>
+  <si>
+    <t>Thao</t>
+  </si>
+  <si>
+    <t>Relevant papers will include Drain PK</t>
+  </si>
+  <si>
+    <t>Obimbo</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>University of Nairobi</t>
+  </si>
+  <si>
+    <t>Ong</t>
+  </si>
+  <si>
+    <t>Shao-En</t>
+  </si>
+  <si>
+    <t>Panpradist</t>
+  </si>
+  <si>
+    <t>Nuttada</t>
+  </si>
+  <si>
+    <t>Parish</t>
+  </si>
+  <si>
+    <t>Tanya</t>
+  </si>
+  <si>
+    <t>Pepple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kathryn </t>
+  </si>
+  <si>
+    <t>Plumplee</t>
+  </si>
+  <si>
+    <t>Courtney</t>
+  </si>
+  <si>
+    <t>Rais</t>
+  </si>
+  <si>
+    <t>Maham</t>
+  </si>
+  <si>
+    <t>Seatle Children's Research Institute</t>
+  </si>
+  <si>
+    <t>Ross</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Saha</t>
+  </si>
+  <si>
+    <t>Aparajita</t>
+  </si>
+  <si>
+    <t>Relevant papers will include Shah JA</t>
+  </si>
+  <si>
+    <t>Seshadri</t>
+  </si>
+  <si>
+    <t>Chetan</t>
+  </si>
+  <si>
+    <t>Shah</t>
+  </si>
+  <si>
+    <t>Javeed</t>
+  </si>
+  <si>
+    <t>Shapiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adrienne </t>
+  </si>
+  <si>
+    <t>Shaporifar</t>
+  </si>
+  <si>
+    <t>Shima</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Manuja</t>
+  </si>
+  <si>
+    <t>Relevant papers will include Patel SN</t>
+  </si>
+  <si>
+    <t>Sherman</t>
+  </si>
+  <si>
+    <t>Simmons</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Sorri</t>
+  </si>
+  <si>
+    <t>Yoseph</t>
+  </si>
+  <si>
     <t>Subramanian</t>
   </si>
   <si>
     <t>Naeha</t>
   </si>
   <si>
-    <t>Associate Professor or Member</t>
-  </si>
-  <si>
-    <t>Nduba</t>
-  </si>
-  <si>
-    <t>Videlis</t>
-  </si>
-  <si>
-    <t>Kenya Medical Research Institute</t>
-  </si>
-  <si>
-    <t>Mayanja-Kizza</t>
-  </si>
-  <si>
-    <t>Harriet</t>
-  </si>
-  <si>
-    <t>Makerere University</t>
-  </si>
-  <si>
-    <t>Narita</t>
-  </si>
-  <si>
-    <t>Masa</t>
-  </si>
-  <si>
-    <t>Public Health Seattle/King County</t>
-  </si>
-  <si>
-    <t>Sorri</t>
-  </si>
-  <si>
-    <t>Yoseph</t>
-  </si>
-  <si>
-    <t>Anterasian</t>
-  </si>
-  <si>
-    <t>Christine</t>
-  </si>
-  <si>
-    <t>Seattle Children's Hospital</t>
-  </si>
-  <si>
-    <t>Assistant Professor or Member</t>
-  </si>
-  <si>
-    <t>Aitchison</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Seattle Children's Research Institute</t>
-  </si>
-  <si>
-    <t>Coler</t>
-  </si>
-  <si>
-    <t>Rhea</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Duffy</t>
-  </si>
-  <si>
-    <t>Fergal</t>
-  </si>
-  <si>
-    <t>Gern</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>Acting or Clinical Instructor</t>
-  </si>
-  <si>
-    <t>Harrington</t>
-  </si>
-  <si>
-    <t>Whitney</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Hernandez</t>
-  </si>
-  <si>
-    <t>Rafael</t>
-  </si>
-  <si>
-    <t>Jaspan</t>
-  </si>
-  <si>
-    <t>Heather</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>Shuyi</t>
-  </si>
-  <si>
-    <t>Need to search with Affiliation</t>
-  </si>
-  <si>
-    <t>McDermott</t>
-  </si>
-  <si>
-    <t>Suzanne</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Parish</t>
-  </si>
-  <si>
-    <t>Tanya</t>
+    <t>Trehan</t>
+  </si>
+  <si>
+    <t>Indi</t>
   </si>
   <si>
     <t>Urdahl</t>
   </si>
   <si>
     <t>Kevin</t>
-  </si>
-  <si>
-    <t>Obimbo</t>
-  </si>
-  <si>
-    <t>Elizabeth</t>
-  </si>
-  <si>
-    <t>University of Nairobi</t>
-  </si>
-  <si>
-    <t>Abernethy</t>
-  </si>
-  <si>
-    <t>Neil</t>
-  </si>
-  <si>
-    <t>University of Washington</t>
-  </si>
-  <si>
-    <t>Attia</t>
-  </si>
-  <si>
-    <t>Engi</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Bender Ignacio</t>
-  </si>
-  <si>
-    <t>Rachel</t>
-  </si>
-  <si>
-    <t>Buckner</t>
-  </si>
-  <si>
-    <t>Frederick</t>
-  </si>
-  <si>
-    <t>Cangelosi</t>
-  </si>
-  <si>
-    <t>Gerard</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Celum</t>
-  </si>
-  <si>
-    <t>Connie</t>
-  </si>
-  <si>
-    <t>Chohan</t>
-  </si>
-  <si>
-    <t>Bhavna</t>
-  </si>
-  <si>
-    <t>Connolly</t>
-  </si>
-  <si>
-    <t>Cowan</t>
-  </si>
-  <si>
-    <t>Fan</t>
-  </si>
-  <si>
-    <t>Erkang</t>
-  </si>
-  <si>
-    <t>Relevant papers will always include FS Buckner</t>
-  </si>
-  <si>
-    <t>Gerner</t>
-  </si>
-  <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Ghassemieh</t>
-  </si>
-  <si>
-    <t>Bijan</t>
-  </si>
-  <si>
-    <t>Gottlieb</t>
-  </si>
-  <si>
-    <t>Geoffrey</t>
-  </si>
-  <si>
-    <t>Graham</t>
-  </si>
-  <si>
-    <t>Susan</t>
-  </si>
-  <si>
-    <t>Grundner</t>
-  </si>
-  <si>
-    <t>Christoph</t>
-  </si>
-  <si>
-    <t>Hawn</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Horne</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Iribarren</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>John-Stewart</t>
-  </si>
-  <si>
-    <t>Grace</t>
-  </si>
-  <si>
-    <t>Kaushansky</t>
-  </si>
-  <si>
-    <t>Alexis</t>
-  </si>
-  <si>
-    <t>Kerani</t>
-  </si>
-  <si>
-    <t>Roxanne</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Koelle</t>
-  </si>
-  <si>
-    <t>LaCourse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sylvia </t>
-  </si>
-  <si>
-    <t>Liles</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Conrad</t>
-  </si>
-  <si>
-    <t>Lutz</t>
-  </si>
-  <si>
-    <t>Barry</t>
-  </si>
-  <si>
-    <t>Ong</t>
-  </si>
-  <si>
-    <t>Shao</t>
-  </si>
-  <si>
-    <t>Panpradist</t>
-  </si>
-  <si>
-    <t>Nuttada</t>
-  </si>
-  <si>
-    <t>Postdoctoral Trainee (Lab-based or Clinical Fellow)</t>
-  </si>
-  <si>
-    <t>Pepple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kathryn </t>
-  </si>
-  <si>
-    <t>Ross</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
-    <t>Seshadri</t>
-  </si>
-  <si>
-    <t>Chetan</t>
-  </si>
-  <si>
-    <t>Shah</t>
-  </si>
-  <si>
-    <t>Javeed</t>
-  </si>
-  <si>
-    <t>Shapiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adrienne </t>
-  </si>
-  <si>
-    <t>Sherman</t>
-  </si>
-  <si>
-    <t>Simmons</t>
-  </si>
-  <si>
-    <t>Jason</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Trehan</t>
-  </si>
-  <si>
-    <t>Indi</t>
   </si>
   <si>
     <t>Wald</t>
@@ -540,7 +693,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -556,6 +709,11 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -606,7 +764,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -644,6 +802,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1806,10 +1973,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1822,7 +1989,7 @@
     <col min="7" max="16384" width="8.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" customHeight="1">
+    <row r="1" spans="1:6" ht="12.75" hidden="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +2016,7 @@
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1859,18 +2026,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:6" ht="20.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>14</v>
@@ -1880,81 +2045,77 @@
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -1964,559 +2125,571 @@
       <c r="B9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="C9" s="7"/>
       <c r="D9" s="5" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="7"/>
       <c r="D11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>40</v>
+      </c>
       <c r="D12" s="5" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="5" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="D14" s="5" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="D15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>52</v>
+        <v>13</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>14</v>
+      <c r="D16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>30</v>
+        <v>55</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>63</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="5" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>67</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="5" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>67</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C21" s="7"/>
       <c r="D21" s="5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="D23" s="5" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="D25" s="5" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>78</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="C27" s="7"/>
       <c r="D27" s="5" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="F27" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="5" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>91</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C29" s="7"/>
       <c r="D29" s="5" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="7"/>
+        <v>89</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="D30" s="5" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="5" t="s">
-        <v>88</v>
+        <v>99</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="7"/>
+        <v>101</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="D36" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>52</v>
+        <v>13</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="7"/>
+        <v>103</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="D37" s="5" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>107</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>110</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C38" s="7"/>
       <c r="D38" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>37</v>
+        <v>13</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>37</v>
+        <v>9</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42" s="7"/>
+        <v>116</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="D42" s="5" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>14</v>
@@ -2524,233 +2697,239 @@
     </row>
     <row r="44" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>30</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C44" s="7"/>
       <c r="D44" s="5" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="7"/>
+        <v>121</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="D45" s="5" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="5" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="5" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="D48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A49" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="B49" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A50" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A49" s="4" t="s">
+      <c r="B50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E49" s="5" t="s">
+      <c r="D50" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A51" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A52" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A53" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A54" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A50" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A51" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A52" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A53" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B53" s="6" t="s">
+    <row r="55" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A55" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A54" s="4" t="s">
+      <c r="B55" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="C55" s="7"/>
+      <c r="D55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E54" s="5" t="s">
+    </row>
+    <row r="56" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A56" s="4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A55" s="4" t="s">
+      <c r="B56" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="C56" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A56" s="4" t="s">
+      <c r="D56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B56" s="5" t="s">
+    </row>
+    <row r="57" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A57" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A57" s="4" t="s">
+      <c r="B57" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="5" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="20.100000000000001" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>152</v>
       </c>
@@ -2758,67 +2937,65 @@
         <v>153</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="20.100000000000001" customHeight="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="6" t="s">
         <v>155</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="20.100000000000001" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>156</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="20.100000000000001" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>159</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C61" s="7"/>
       <c r="D61" s="5" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="20.100000000000001" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>160</v>
       </c>
@@ -2827,47 +3004,422 @@
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="5" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="20.100000000000001" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>163</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="5" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="20.100000000000001" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="4" t="s">
         <v>164</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C64" s="6" t="s">
         <v>165</v>
       </c>
+      <c r="C64" s="8"/>
       <c r="D64" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E64" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A65" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A66" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A67" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="68" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A68" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" s="7"/>
+      <c r="D68" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A69" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C69" s="7"/>
+      <c r="D69" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A70" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A71" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A72" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A73" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A74" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A75" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C75" s="7"/>
+      <c r="D75" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A76" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A77" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A78" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A79" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A80" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A81" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A82" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C82" s="7"/>
+      <c r="D82" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A83" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C83" s="7"/>
+      <c r="D83" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A84" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C84" s="7"/>
+      <c r="D84" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A85" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A86" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C86" s="7"/>
+      <c r="D86" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A87" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
-    <sortCondition ref="D2:D64"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F87">
+    <sortCondition ref="A41:A87"/>
   </sortState>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
@@ -2878,6 +3430,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="21ca8ef8-3399-4ca3-b62e-f30736ef5ac0">
+      <UserInfo>
+        <DisplayName>Jordan McCrary</DisplayName>
+        <AccountId>35</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="ab06a5aa-8e31-4bdb-9b13-38c58a92ec8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3b350f9-b33f-4a54-b159-0ef6ff0a239a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004FBFC947EB4B81499DC00F91BCC164EF" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ddcb7a999dfa0e72c3d6e3779556a454">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3b350f9-b33f-4a54-b159-0ef6ff0a239a" xmlns:ns3="ab06a5aa-8e31-4bdb-9b13-38c58a92ec8a" xmlns:ns4="21ca8ef8-3399-4ca3-b62e-f30736ef5ac0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a07f0f6eff6615e668ffab45792588a" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="d3b350f9-b33f-4a54-b159-0ef6ff0a239a"/>
@@ -3137,24 +3707,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="21ca8ef8-3399-4ca3-b62e-f30736ef5ac0">
-      <UserInfo>
-        <DisplayName>Jordan McCrary</DisplayName>
-        <AccountId>35</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="ab06a5aa-8e31-4bdb-9b13-38c58a92ec8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3b350f9-b33f-4a54-b159-0ef6ff0a239a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3165,11 +3717,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F019B846-7F6B-499C-A2AD-578DE2BFE9CD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC8EA8E4-2D52-4F0D-A9D2-F0D876498797}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC8EA8E4-2D52-4F0D-A9D2-F0D876498797}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F019B846-7F6B-499C-A2AD-578DE2BFE9CD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>